<commit_message>
feat: Add responsive CSS
</commit_message>
<xml_diff>
--- a/issueLog.xlsx
+++ b/issueLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kirei Yume\Documents\Atom\Memory-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD57502-F835-465E-9C02-7E24BCD25E54}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C35985-5767-444F-B7B8-2DCC97812F71}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{F0E7D85A-DC76-455D-B1BD-81FAD8BCA67E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>issue log</t>
   </si>
@@ -48,6 +48,36 @@
   </si>
   <si>
     <t xml:space="preserve">either delay or add more variable storage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">function </t>
+  </si>
+  <si>
+    <t xml:space="preserve">check </t>
+  </si>
+  <si>
+    <t xml:space="preserve">some cards stay flipped even if they don't match </t>
+  </si>
+  <si>
+    <t xml:space="preserve">flippping animation happens faster when clicking faster </t>
+  </si>
+  <si>
+    <t xml:space="preserve">seems to match incorrectly when clicking faster </t>
+  </si>
+  <si>
+    <t xml:space="preserve">flipping doesn't happen in the right order </t>
+  </si>
+  <si>
+    <t xml:space="preserve">footer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">make it absolute position </t>
+  </si>
+  <si>
+    <t xml:space="preserve">media queries </t>
+  </si>
+  <si>
+    <t xml:space="preserve">stars function for the win page does not work properly </t>
   </si>
 </sst>
 </file>
@@ -402,27 +432,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB40BD90-0B27-4F83-BEA8-061DA1474435}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="141.5703125" customWidth="1"/>
     <col min="2" max="2" width="57" customWidth="1"/>
+    <col min="3" max="3" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -430,17 +464,58 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Change star function
</commit_message>
<xml_diff>
--- a/issueLog.xlsx
+++ b/issueLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kirei Yume\Documents\Atom\Memory-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C35985-5767-444F-B7B8-2DCC97812F71}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71881811-6138-4ADD-B113-26A4DC598152}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{F0E7D85A-DC76-455D-B1BD-81FAD8BCA67E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>issue log</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t xml:space="preserve">stars function for the win page does not work properly </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dynamically change position with event listener </t>
   </si>
 </sst>
 </file>
@@ -432,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB40BD90-0B27-4F83-BEA8-061DA1474435}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,6 +521,11 @@
         <v>16</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>